<commit_message>
Adding patchmethod use case
</commit_message>
<xml_diff>
--- a/Utilities/data.xlsx
+++ b/Utilities/data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\.m2\Intellij\SampleRESTAPIFramework\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8553A9F-F605-4513-BF6C-6D6D63352B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874A32AC-4DC5-4F57-AF9C-0612E3BB7137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Url" sheetId="1" r:id="rId1"/>
     <sheet name="AddUser" sheetId="3" r:id="rId2"/>
+    <sheet name="UpdateUser" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>UserId</t>
   </si>
@@ -53,6 +54,12 @@
   </si>
   <si>
     <t>male</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>7354294</t>
   </si>
 </sst>
 </file>
@@ -401,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{959A6FFF-EBE5-427A-B201-5EB72D367F5A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -438,4 +445,41 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4EB8EE6-7756-40D7-BFCD-7E9A2FC488F0}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>